<commit_message>
Creating file for the report
</commit_message>
<xml_diff>
--- a/Goryachaya_trubka.xlsx
+++ b/Goryachaya_trubka.xlsx
@@ -176,12 +176,52 @@
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent4"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="0.1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Лист1!$A$5:$A$46</c:f>
@@ -488,7 +528,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
@@ -2388,10 +2428,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>

</xml_diff>